<commit_message>
Req.001 began + Timetable
</commit_message>
<xml_diff>
--- a/doc/Projekt Planung.xlsx
+++ b/doc/Projekt Planung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Texas_Hold'em_Casual\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B26152AC-59AF-428D-8584-24FA4332459D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8312809-C717-4558-BF37-930C5B35FA6C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitplanung!$A$1:$T$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
   <si>
     <t>Nr.</t>
   </si>
@@ -227,40 +228,37 @@
     <t>-</t>
   </si>
   <si>
-    <t>Aussicht von Tisch und Karten machen</t>
-  </si>
-  <si>
-    <t>2 Karten für alle 5 Spieler Austeilen</t>
-  </si>
-  <si>
-    <t>Mindest Mise machen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mise Erhöhung </t>
-  </si>
-  <si>
-    <t>Karte wegwerfen</t>
-  </si>
-  <si>
-    <t>gemeinsame Karten legen</t>
-  </si>
-  <si>
-    <t>gemeinsame Karten brennen</t>
-  </si>
-  <si>
-    <t>Sieg/Verlust (Ende das Spiels)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mise geben </t>
-  </si>
-  <si>
-    <t>Karten Zeigen</t>
-  </si>
-  <si>
     <t>20.12.</t>
   </si>
   <si>
     <t>Texas holdem casual</t>
+  </si>
+  <si>
+    <t>F.REQ.001</t>
+  </si>
+  <si>
+    <t>F.REQ.002</t>
+  </si>
+  <si>
+    <t>F.REQ.003</t>
+  </si>
+  <si>
+    <t>F.REQ.004</t>
+  </si>
+  <si>
+    <t>F.REQ.005</t>
+  </si>
+  <si>
+    <t>F.REQ.006</t>
+  </si>
+  <si>
+    <t>F.REQ.007</t>
+  </si>
+  <si>
+    <t>F.REQ.008</t>
+  </si>
+  <si>
+    <t>F.REQ.009</t>
   </si>
 </sst>
 </file>
@@ -375,7 +373,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,6 +468,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="49">
     <border>
@@ -1114,7 +1118,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1431,14 +1435,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1469,6 +1465,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1483,10 +1483,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9999"/>
       <color rgb="FFFFCCCC"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFFF5050"/>
-      <color rgb="FFFF9999"/>
       <color rgb="FFFFFFCC"/>
     </mruColors>
   </colors>
@@ -1576,7 +1576,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -1647,10 +1647,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2157,8 +2157,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2174,7 +2174,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2477,88 +2477,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="96" t="s">
+      <c r="C7" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="96"/>
+      <c r="D7" s="94"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="95" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="97"/>
-      <c r="I7" s="97"/>
-      <c r="J7" s="97"/>
-      <c r="K7" s="97"/>
-      <c r="L7" s="97"/>
-      <c r="M7" s="98"/>
-      <c r="N7" s="97" t="s">
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="97"/>
-      <c r="P7" s="97"/>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="97"/>
-      <c r="S7" s="97"/>
-      <c r="T7" s="98"/>
-      <c r="U7" s="97" t="s">
+      <c r="O7" s="95"/>
+      <c r="P7" s="95"/>
+      <c r="Q7" s="95"/>
+      <c r="R7" s="95"/>
+      <c r="S7" s="95"/>
+      <c r="T7" s="96"/>
+      <c r="U7" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="97"/>
-      <c r="W7" s="97"/>
-      <c r="X7" s="97"/>
-      <c r="Y7" s="97"/>
-      <c r="Z7" s="97"/>
-      <c r="AA7" s="98"/>
-      <c r="AB7" s="99" t="s">
+      <c r="V7" s="95"/>
+      <c r="W7" s="95"/>
+      <c r="X7" s="95"/>
+      <c r="Y7" s="95"/>
+      <c r="Z7" s="95"/>
+      <c r="AA7" s="96"/>
+      <c r="AB7" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="AC7" s="97"/>
-      <c r="AD7" s="97"/>
-      <c r="AE7" s="97"/>
-      <c r="AF7" s="97"/>
-      <c r="AG7" s="97"/>
-      <c r="AH7" s="98"/>
-      <c r="AI7" s="97" t="s">
+      <c r="AC7" s="95"/>
+      <c r="AD7" s="95"/>
+      <c r="AE7" s="95"/>
+      <c r="AF7" s="95"/>
+      <c r="AG7" s="95"/>
+      <c r="AH7" s="96"/>
+      <c r="AI7" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="AJ7" s="97"/>
-      <c r="AK7" s="97"/>
-      <c r="AL7" s="97"/>
-      <c r="AM7" s="97"/>
-      <c r="AN7" s="97"/>
-      <c r="AO7" s="98"/>
-      <c r="AP7" s="99" t="s">
+      <c r="AJ7" s="95"/>
+      <c r="AK7" s="95"/>
+      <c r="AL7" s="95"/>
+      <c r="AM7" s="95"/>
+      <c r="AN7" s="95"/>
+      <c r="AO7" s="96"/>
+      <c r="AP7" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="AQ7" s="97"/>
-      <c r="AR7" s="97"/>
-      <c r="AS7" s="97"/>
-      <c r="AT7" s="97"/>
-      <c r="AU7" s="97"/>
-      <c r="AV7" s="98"/>
-      <c r="AW7" s="97" t="s">
+      <c r="AQ7" s="95"/>
+      <c r="AR7" s="95"/>
+      <c r="AS7" s="95"/>
+      <c r="AT7" s="95"/>
+      <c r="AU7" s="95"/>
+      <c r="AV7" s="96"/>
+      <c r="AW7" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="AX7" s="97"/>
-      <c r="AY7" s="97"/>
-      <c r="AZ7" s="97"/>
-      <c r="BA7" s="97"/>
-      <c r="BB7" s="97"/>
-      <c r="BC7" s="98"/>
-      <c r="BD7" s="99" t="s">
+      <c r="AX7" s="95"/>
+      <c r="AY7" s="95"/>
+      <c r="AZ7" s="95"/>
+      <c r="BA7" s="95"/>
+      <c r="BB7" s="95"/>
+      <c r="BC7" s="96"/>
+      <c r="BD7" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="BE7" s="97"/>
-      <c r="BF7" s="97"/>
-      <c r="BG7" s="97"/>
-      <c r="BH7" s="97"/>
-      <c r="BI7" s="97"/>
-      <c r="BJ7" s="100"/>
+      <c r="BE7" s="95"/>
+      <c r="BF7" s="95"/>
+      <c r="BG7" s="95"/>
+      <c r="BH7" s="95"/>
+      <c r="BI7" s="95"/>
+      <c r="BJ7" s="98"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -3133,7 +3133,7 @@
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3204,7 +3204,7 @@
       <c r="C15" s="49"/>
       <c r="D15" s="83">
         <f>SUM(G15:BJ15)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="89" t="s">
@@ -3213,7 +3213,9 @@
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
       <c r="I15" s="68"/>
-      <c r="J15" s="87"/>
+      <c r="J15" s="87">
+        <v>5</v>
+      </c>
       <c r="K15" s="63"/>
       <c r="L15" s="57"/>
       <c r="M15" s="58"/>
@@ -3416,11 +3418,11 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3568,7 +3570,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3577,7 +3579,9 @@
       <c r="G20" s="59"/>
       <c r="H20" s="60"/>
       <c r="I20" s="55"/>
-      <c r="J20" s="68"/>
+      <c r="J20" s="68">
+        <v>2</v>
+      </c>
       <c r="K20" s="63"/>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
@@ -3636,7 +3640,7 @@
         <v>303</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C21" s="49">
         <v>6</v>
@@ -3655,14 +3659,14 @@
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
-      <c r="K21" s="56"/>
+      <c r="K21" s="63"/>
       <c r="L21" s="57"/>
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
       <c r="P21" s="68"/>
-      <c r="Q21" s="68"/>
-      <c r="R21" s="95"/>
+      <c r="Q21" s="93"/>
+      <c r="R21" s="91"/>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
       <c r="U21" s="59"/>
@@ -3713,7 +3717,7 @@
         <v>304</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C22" s="49">
         <v>4</v>
@@ -3735,9 +3739,9 @@
       <c r="M22" s="58"/>
       <c r="N22" s="59"/>
       <c r="O22" s="60"/>
-      <c r="P22" s="55"/>
+      <c r="P22" s="68"/>
       <c r="Q22" s="55"/>
-      <c r="R22" s="63"/>
+      <c r="R22" s="91"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
@@ -3788,7 +3792,7 @@
         <v>305</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C23" s="49">
         <v>4</v>
@@ -3801,7 +3805,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="51" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G23" s="59"/>
       <c r="H23" s="60"/>
@@ -3812,15 +3816,15 @@
       <c r="M23" s="58"/>
       <c r="N23" s="59"/>
       <c r="O23" s="60"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="61"/>
-      <c r="R23" s="63"/>
+      <c r="P23" s="90"/>
+      <c r="Q23" s="90"/>
+      <c r="R23" s="91"/>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="90"/>
-      <c r="X23" s="94"/>
+      <c r="W23" s="85"/>
+      <c r="X23" s="85"/>
       <c r="Y23" s="56"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
@@ -3865,7 +3869,7 @@
         <v>306</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C24" s="49">
         <v>7</v>
@@ -3888,14 +3892,14 @@
       <c r="N24" s="59"/>
       <c r="O24" s="60"/>
       <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
-      <c r="R24" s="91"/>
+      <c r="Q24" s="68"/>
+      <c r="R24" s="103"/>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
       <c r="W24" s="93"/>
-      <c r="X24" s="68"/>
+      <c r="X24" s="93"/>
       <c r="Y24" s="91"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
@@ -3940,7 +3944,7 @@
         <v>307</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C25" s="49">
         <v>4</v>
@@ -3964,13 +3968,13 @@
       <c r="O25" s="60"/>
       <c r="P25" s="55"/>
       <c r="Q25" s="55"/>
-      <c r="R25" s="91"/>
+      <c r="R25" s="63"/>
       <c r="S25" s="57"/>
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
       <c r="V25" s="60"/>
-      <c r="W25" s="55"/>
-      <c r="X25" s="68"/>
+      <c r="W25" s="68"/>
+      <c r="X25" s="93"/>
       <c r="Y25" s="56"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
@@ -4015,7 +4019,7 @@
         <v>308</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C26" s="49">
         <v>1</v>
@@ -4090,7 +4094,7 @@
         <v>309</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C27" s="49">
         <v>1</v>
@@ -4121,7 +4125,7 @@
       <c r="V27" s="60"/>
       <c r="W27" s="55"/>
       <c r="X27" s="68"/>
-      <c r="Y27" s="63"/>
+      <c r="Y27" s="91"/>
       <c r="Z27" s="57"/>
       <c r="AA27" s="58"/>
       <c r="AB27" s="59"/>
@@ -4165,7 +4169,7 @@
         <v>310</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C28" s="49">
         <v>1</v>
@@ -4240,7 +4244,7 @@
         <v>311</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C29" s="49">
         <v>1</v>
@@ -4290,7 +4294,7 @@
       <c r="AO29" s="58"/>
       <c r="AP29" s="71"/>
       <c r="AQ29" s="72"/>
-      <c r="AR29" s="55"/>
+      <c r="AR29" s="68"/>
       <c r="AS29" s="55"/>
       <c r="AT29" s="56"/>
       <c r="AU29" s="57"/>
@@ -4314,19 +4318,13 @@
       <c r="A30" s="12">
         <v>312</v>
       </c>
-      <c r="B30" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" s="49">
-        <v>1</v>
-      </c>
+      <c r="B30" s="46"/>
+      <c r="C30" s="49"/>
       <c r="D30" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="50">
-        <v>2</v>
-      </c>
+      <c r="E30" s="50"/>
       <c r="F30" s="51"/>
       <c r="G30" s="69"/>
       <c r="H30" s="70"/>
@@ -4346,7 +4344,7 @@
       <c r="V30" s="70"/>
       <c r="W30" s="55"/>
       <c r="X30" s="55"/>
-      <c r="Y30" s="63"/>
+      <c r="Y30" s="103"/>
       <c r="Z30" s="57"/>
       <c r="AA30" s="58"/>
       <c r="AB30" s="69"/>
@@ -5253,11 +5251,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5275,7 +5273,7 @@
       </c>
       <c r="J43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
@@ -5532,10 +5530,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="104"/>
+      <c r="B2" s="102"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5544,11 +5542,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="101" t="str">
+      <c r="A3" s="99" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="102"/>
+      <c r="B3" s="100"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>5</v>
@@ -5561,45 +5559,45 @@
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="101" t="str">
+      <c r="A4" s="99" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="102"/>
+      <c r="B4" s="100"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>0</v>
       </c>
       <c r="D4" s="80">
         <f>Zeitplanung!D14</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="101" t="str">
+      <c r="A5" s="99" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="102"/>
+      <c r="B5" s="100"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="101" t="str">
+      <c r="A6" s="99" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="102"/>
+      <c r="B6" s="100"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>3</v>
@@ -5611,11 +5609,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="101" t="str">
+      <c r="A7" s="99" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="102"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>0</v>
@@ -5627,11 +5625,11 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="101" t="str">
+      <c r="A8" s="99" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="102"/>
+      <c r="B8" s="100"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
         <v>0</v>

</xml_diff>

<commit_message>
created deck of cards + show a card
</commit_message>
<xml_diff>
--- a/doc/Projekt Planung.xlsx
+++ b/doc/Projekt Planung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Texas_Hold'em_Casual\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8312809-C717-4558-BF37-930C5B35FA6C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E025C2E-A56E-4341-9D2D-0D0E4D26F514}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitplanung!$A$1:$T$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -76,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
   <si>
     <t>Nr.</t>
   </si>
@@ -228,9 +227,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>20.12.</t>
-  </si>
-  <si>
     <t>Texas holdem casual</t>
   </si>
   <si>
@@ -259,6 +255,12 @@
   </si>
   <si>
     <t>F.REQ.009</t>
+  </si>
+  <si>
+    <t>14.12.</t>
+  </si>
+  <si>
+    <t>21.12.</t>
   </si>
 </sst>
 </file>
@@ -1435,6 +1437,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1465,10 +1471,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2158,7 +2160,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="F24" sqref="F24:R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2174,7 +2176,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2477,88 +2479,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="94"/>
+      <c r="D7" s="95"/>
       <c r="E7" s="28" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="95" t="s">
+      <c r="G7" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="95" t="s">
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="95"/>
-      <c r="P7" s="95"/>
-      <c r="Q7" s="95"/>
-      <c r="R7" s="95"/>
-      <c r="S7" s="95"/>
-      <c r="T7" s="96"/>
-      <c r="U7" s="95" t="s">
+      <c r="O7" s="96"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="96"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="97"/>
+      <c r="U7" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="95"/>
-      <c r="W7" s="95"/>
-      <c r="X7" s="95"/>
-      <c r="Y7" s="95"/>
-      <c r="Z7" s="95"/>
-      <c r="AA7" s="96"/>
-      <c r="AB7" s="97" t="s">
+      <c r="V7" s="96"/>
+      <c r="W7" s="96"/>
+      <c r="X7" s="96"/>
+      <c r="Y7" s="96"/>
+      <c r="Z7" s="96"/>
+      <c r="AA7" s="97"/>
+      <c r="AB7" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="AC7" s="95"/>
-      <c r="AD7" s="95"/>
-      <c r="AE7" s="95"/>
-      <c r="AF7" s="95"/>
-      <c r="AG7" s="95"/>
-      <c r="AH7" s="96"/>
-      <c r="AI7" s="95" t="s">
+      <c r="AC7" s="96"/>
+      <c r="AD7" s="96"/>
+      <c r="AE7" s="96"/>
+      <c r="AF7" s="96"/>
+      <c r="AG7" s="96"/>
+      <c r="AH7" s="97"/>
+      <c r="AI7" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="AJ7" s="95"/>
-      <c r="AK7" s="95"/>
-      <c r="AL7" s="95"/>
-      <c r="AM7" s="95"/>
-      <c r="AN7" s="95"/>
-      <c r="AO7" s="96"/>
-      <c r="AP7" s="97" t="s">
+      <c r="AJ7" s="96"/>
+      <c r="AK7" s="96"/>
+      <c r="AL7" s="96"/>
+      <c r="AM7" s="96"/>
+      <c r="AN7" s="96"/>
+      <c r="AO7" s="97"/>
+      <c r="AP7" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="AQ7" s="95"/>
-      <c r="AR7" s="95"/>
-      <c r="AS7" s="95"/>
-      <c r="AT7" s="95"/>
-      <c r="AU7" s="95"/>
-      <c r="AV7" s="96"/>
-      <c r="AW7" s="95" t="s">
+      <c r="AQ7" s="96"/>
+      <c r="AR7" s="96"/>
+      <c r="AS7" s="96"/>
+      <c r="AT7" s="96"/>
+      <c r="AU7" s="96"/>
+      <c r="AV7" s="97"/>
+      <c r="AW7" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="AX7" s="95"/>
-      <c r="AY7" s="95"/>
-      <c r="AZ7" s="95"/>
-      <c r="BA7" s="95"/>
-      <c r="BB7" s="95"/>
-      <c r="BC7" s="96"/>
-      <c r="BD7" s="97" t="s">
+      <c r="AX7" s="96"/>
+      <c r="AY7" s="96"/>
+      <c r="AZ7" s="96"/>
+      <c r="BA7" s="96"/>
+      <c r="BB7" s="96"/>
+      <c r="BC7" s="97"/>
+      <c r="BD7" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="BE7" s="95"/>
-      <c r="BF7" s="95"/>
-      <c r="BG7" s="95"/>
-      <c r="BH7" s="95"/>
-      <c r="BI7" s="95"/>
-      <c r="BJ7" s="98"/>
+      <c r="BE7" s="96"/>
+      <c r="BF7" s="96"/>
+      <c r="BG7" s="96"/>
+      <c r="BH7" s="96"/>
+      <c r="BI7" s="96"/>
+      <c r="BJ7" s="99"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
@@ -3640,7 +3642,7 @@
         <v>303</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="49">
         <v>6</v>
@@ -3652,9 +3654,7 @@
       <c r="E21" s="50">
         <v>1</v>
       </c>
-      <c r="F21" s="52">
-        <v>14.12</v>
-      </c>
+      <c r="F21" s="52"/>
       <c r="G21" s="59"/>
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
@@ -3717,7 +3717,7 @@
         <v>304</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="49">
         <v>4</v>
@@ -3792,7 +3792,7 @@
         <v>305</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="49">
         <v>4</v>
@@ -3804,9 +3804,7 @@
       <c r="E23" s="50">
         <v>1</v>
       </c>
-      <c r="F23" s="51" t="s">
-        <v>50</v>
-      </c>
+      <c r="F23" s="51"/>
       <c r="G23" s="59"/>
       <c r="H23" s="60"/>
       <c r="I23" s="61"/>
@@ -3869,7 +3867,7 @@
         <v>306</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="49">
         <v>7</v>
@@ -3881,7 +3879,9 @@
       <c r="E24" s="50">
         <v>1</v>
       </c>
-      <c r="F24" s="51"/>
+      <c r="F24" s="51" t="s">
+        <v>60</v>
+      </c>
       <c r="G24" s="59"/>
       <c r="H24" s="60"/>
       <c r="I24" s="55"/>
@@ -3893,7 +3893,7 @@
       <c r="O24" s="60"/>
       <c r="P24" s="55"/>
       <c r="Q24" s="68"/>
-      <c r="R24" s="103"/>
+      <c r="R24" s="94"/>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
@@ -3944,7 +3944,7 @@
         <v>307</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="49">
         <v>4</v>
@@ -4019,7 +4019,7 @@
         <v>308</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="49">
         <v>1</v>
@@ -4094,7 +4094,7 @@
         <v>309</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="49">
         <v>1</v>
@@ -4169,7 +4169,7 @@
         <v>310</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="49">
         <v>1</v>
@@ -4244,7 +4244,7 @@
         <v>311</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="49">
         <v>1</v>
@@ -4325,7 +4325,9 @@
         <v>0</v>
       </c>
       <c r="E30" s="50"/>
-      <c r="F30" s="51"/>
+      <c r="F30" s="51" t="s">
+        <v>61</v>
+      </c>
       <c r="G30" s="69"/>
       <c r="H30" s="70"/>
       <c r="I30" s="55"/>
@@ -4344,7 +4346,7 @@
       <c r="V30" s="70"/>
       <c r="W30" s="55"/>
       <c r="X30" s="55"/>
-      <c r="Y30" s="103"/>
+      <c r="Y30" s="94"/>
       <c r="Z30" s="57"/>
       <c r="AA30" s="58"/>
       <c r="AB30" s="69"/>
@@ -5530,10 +5532,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="102"/>
+      <c r="B2" s="103"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5542,11 +5544,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="99" t="str">
+      <c r="A3" s="100" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="100"/>
+      <c r="B3" s="101"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>5</v>
@@ -5559,11 +5561,11 @@
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99" t="str">
+      <c r="A4" s="100" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="100"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>0</v>
@@ -5576,11 +5578,11 @@
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="str">
+      <c r="A5" s="100" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="100"/>
+      <c r="B5" s="101"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>31</v>
@@ -5593,11 +5595,11 @@
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="99" t="str">
+      <c r="A6" s="100" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>3</v>
@@ -5609,11 +5611,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="99" t="str">
+      <c r="A7" s="100" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="100"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>0</v>
@@ -5625,11 +5627,11 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="str">
+      <c r="A8" s="100" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="100"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
         <v>0</v>

</xml_diff>

<commit_message>
new frame with javafx
</commit_message>
<xml_diff>
--- a/doc/Projekt Planung.xlsx
+++ b/doc/Projekt Planung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Texas_Hold'em_Casual\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E025C2E-A56E-4341-9D2D-0D0E4D26F514}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A679AAAB-DD48-408A-8725-5EB868253DA6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1578,7 +1578,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -1646,13 +1646,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2159,8 +2159,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:R24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -2995,7 +2995,9 @@
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="63"/>
+      <c r="K12" s="63">
+        <v>1</v>
+      </c>
       <c r="L12" s="57"/>
       <c r="M12" s="58"/>
       <c r="N12" s="59"/>
@@ -3420,11 +3422,11 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3572,7 +3574,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3584,7 +3586,9 @@
       <c r="J20" s="68">
         <v>2</v>
       </c>
-      <c r="K20" s="63"/>
+      <c r="K20" s="63">
+        <v>1</v>
+      </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
@@ -3649,7 +3653,7 @@
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E21" s="50">
         <v>1</v>
@@ -3659,7 +3663,9 @@
       <c r="H21" s="60"/>
       <c r="I21" s="55"/>
       <c r="J21" s="55"/>
-      <c r="K21" s="63"/>
+      <c r="K21" s="63">
+        <v>6</v>
+      </c>
       <c r="L21" s="57"/>
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
@@ -3720,7 +3726,7 @@
         <v>52</v>
       </c>
       <c r="C22" s="49">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
@@ -3795,7 +3801,7 @@
         <v>53</v>
       </c>
       <c r="C23" s="49">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
@@ -3947,7 +3953,7 @@
         <v>55</v>
       </c>
       <c r="C25" s="49">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
@@ -4022,7 +4028,7 @@
         <v>56</v>
       </c>
       <c r="C26" s="49">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
@@ -4097,7 +4103,7 @@
         <v>57</v>
       </c>
       <c r="C27" s="49">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
@@ -4172,7 +4178,7 @@
         <v>58</v>
       </c>
       <c r="C28" s="49">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D28" s="83">
         <f t="shared" si="0"/>
@@ -4247,7 +4253,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="49">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D29" s="83">
         <f t="shared" si="0"/>
@@ -5253,11 +5259,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5279,7 +5285,7 @@
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5555,7 +5561,7 @@
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
@@ -5585,11 +5591,11 @@
       <c r="B5" s="101"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Poker Hands added except two pairs and highcard
</commit_message>
<xml_diff>
--- a/doc/Projekt Planung.xlsx
+++ b/doc/Projekt Planung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Texas_Hold'em_Casual\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED0C1915-97E8-455A-9F75-EC4E8CFDFBB9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2241779B-F37E-49B3-A3A2-7D1AD6F8AEFD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11565" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11568" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1652,10 +1652,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1760,7 +1760,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1769,16 +1769,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>916078</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>26893</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>459442</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>69476</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>322729</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>60512</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2159,22 +2159,22 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AO29" sqref="AO29"/>
+    <sheetView showGridLines="0" topLeftCell="C7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AS27" sqref="AS27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="31.875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="5.25" style="5" customWidth="1"/>
-    <col min="4" max="4" width="5.25" style="13" customWidth="1"/>
-    <col min="5" max="6" width="5.25" style="5" customWidth="1"/>
-    <col min="7" max="62" width="2.25" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.59765625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31.8984375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="5.19921875" style="13" customWidth="1"/>
+    <col min="5" max="6" width="5.19921875" style="5" customWidth="1"/>
+    <col min="7" max="62" width="2.19921875" style="5" customWidth="1"/>
     <col min="63" max="16384" width="12.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" ht="25.2" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>50</v>
       </c>
@@ -2208,7 +2208,7 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:62" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2272,7 +2272,7 @@
       <c r="BI2" s="6"/>
       <c r="BJ2" s="6"/>
     </row>
-    <row r="3" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2338,7 +2338,7 @@
       <c r="BI3" s="6"/>
       <c r="BJ3" s="6"/>
     </row>
-    <row r="4" spans="1:62" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2402,7 +2402,7 @@
       <c r="BI4" s="6"/>
       <c r="BJ4" s="6"/>
     </row>
-    <row r="5" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -2468,7 +2468,7 @@
       <c r="BI5" s="6"/>
       <c r="BJ5" s="6"/>
     </row>
-    <row r="6" spans="1:62" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2476,7 +2476,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
       <c r="C7" s="95" t="s">
@@ -2562,7 +2562,7 @@
       <c r="BI7" s="96"/>
       <c r="BJ7" s="99"/>
     </row>
-    <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
@@ -2748,7 +2748,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>10</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="BI9" s="74"/>
       <c r="BJ9" s="78"/>
     </row>
-    <row r="10" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>101</v>
       </c>
@@ -2896,7 +2896,7 @@
       <c r="BI10" s="57"/>
       <c r="BJ10" s="58"/>
     </row>
-    <row r="11" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>102</v>
       </c>
@@ -2973,7 +2973,7 @@
       <c r="BI11" s="57"/>
       <c r="BJ11" s="58"/>
     </row>
-    <row r="12" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>103</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="BI12" s="57"/>
       <c r="BJ12" s="58"/>
     </row>
-    <row r="13" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>104</v>
       </c>
@@ -3124,7 +3124,7 @@
       <c r="BI13" s="66"/>
       <c r="BJ13" s="67"/>
     </row>
-    <row r="14" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30">
         <v>20</v>
       </c>
@@ -3198,7 +3198,7 @@
       <c r="BI14" s="74"/>
       <c r="BJ14" s="78"/>
     </row>
-    <row r="15" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>201</v>
       </c>
@@ -3273,7 +3273,7 @@
       <c r="BI15" s="57"/>
       <c r="BJ15" s="58"/>
     </row>
-    <row r="16" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>202</v>
       </c>
@@ -3344,7 +3344,7 @@
       <c r="BI16" s="57"/>
       <c r="BJ16" s="58"/>
     </row>
-    <row r="17" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>203</v>
       </c>
@@ -3413,7 +3413,7 @@
       <c r="BI17" s="57"/>
       <c r="BJ17" s="58"/>
     </row>
-    <row r="18" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30">
         <v>30</v>
       </c>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3487,7 +3487,7 @@
       <c r="BI18" s="74"/>
       <c r="BJ18" s="78"/>
     </row>
-    <row r="19" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>301</v>
       </c>
@@ -3562,7 +3562,7 @@
       <c r="BI19" s="57"/>
       <c r="BJ19" s="58"/>
     </row>
-    <row r="20" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>302</v>
       </c>
@@ -3643,7 +3643,7 @@
       <c r="BI20" s="57"/>
       <c r="BJ20" s="58"/>
     </row>
-    <row r="21" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>303</v>
       </c>
@@ -3722,7 +3722,7 @@
       <c r="BI21" s="57"/>
       <c r="BJ21" s="58"/>
     </row>
-    <row r="22" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>304</v>
       </c>
@@ -3734,7 +3734,7 @@
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E22" s="50">
         <v>1</v>
@@ -3762,7 +3762,9 @@
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
-      <c r="W22" s="55"/>
+      <c r="W22" s="55">
+        <v>4</v>
+      </c>
       <c r="X22" s="55"/>
       <c r="Y22" s="56"/>
       <c r="Z22" s="57"/>
@@ -3803,7 +3805,7 @@
       <c r="BI22" s="57"/>
       <c r="BJ22" s="58"/>
     </row>
-    <row r="23" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>305</v>
       </c>
@@ -3878,7 +3880,7 @@
       <c r="BI23" s="57"/>
       <c r="BJ23" s="58"/>
     </row>
-    <row r="24" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>306</v>
       </c>
@@ -3890,7 +3892,7 @@
       </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="50">
         <v>1</v>
@@ -3915,7 +3917,9 @@
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
       <c r="W24" s="93"/>
-      <c r="X24" s="93"/>
+      <c r="X24" s="93">
+        <v>2</v>
+      </c>
       <c r="Y24" s="63"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
@@ -3955,7 +3959,7 @@
       <c r="BI24" s="57"/>
       <c r="BJ24" s="58"/>
     </row>
-    <row r="25" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>307</v>
       </c>
@@ -4032,7 +4036,7 @@
       <c r="BI25" s="57"/>
       <c r="BJ25" s="58"/>
     </row>
-    <row r="26" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>308</v>
       </c>
@@ -4044,7 +4048,7 @@
       </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E26" s="50">
         <v>1</v>
@@ -4066,9 +4070,15 @@
       <c r="T26" s="58"/>
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
-      <c r="W26" s="68"/>
-      <c r="X26" s="68"/>
-      <c r="Y26" s="63"/>
+      <c r="W26" s="68">
+        <v>4</v>
+      </c>
+      <c r="X26" s="68">
+        <v>6</v>
+      </c>
+      <c r="Y26" s="63">
+        <v>6</v>
+      </c>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
       <c r="AB26" s="59"/>
@@ -4087,7 +4097,9 @@
       <c r="AO26" s="58"/>
       <c r="AP26" s="59"/>
       <c r="AQ26" s="60"/>
-      <c r="AR26" s="55"/>
+      <c r="AR26" s="55">
+        <v>4</v>
+      </c>
       <c r="AS26" s="55"/>
       <c r="AT26" s="56"/>
       <c r="AU26" s="57"/>
@@ -4107,7 +4119,7 @@
       <c r="BI26" s="57"/>
       <c r="BJ26" s="58"/>
     </row>
-    <row r="27" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>309</v>
       </c>
@@ -4163,7 +4175,7 @@
       <c r="AP27" s="59"/>
       <c r="AQ27" s="60"/>
       <c r="AR27" s="68"/>
-      <c r="AS27" s="55"/>
+      <c r="AS27" s="68"/>
       <c r="AT27" s="56"/>
       <c r="AU27" s="57"/>
       <c r="AV27" s="58"/>
@@ -4182,7 +4194,7 @@
       <c r="BI27" s="57"/>
       <c r="BJ27" s="58"/>
     </row>
-    <row r="28" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>310</v>
       </c>
@@ -4197,7 +4209,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F28" s="51"/>
       <c r="G28" s="59"/>
@@ -4257,7 +4269,7 @@
       <c r="BI28" s="57"/>
       <c r="BJ28" s="58"/>
     </row>
-    <row r="29" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>311</v>
       </c>
@@ -4272,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="50">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F29" s="51"/>
       <c r="G29" s="71"/>
@@ -4332,7 +4344,7 @@
       <c r="BI29" s="57"/>
       <c r="BJ29" s="58"/>
     </row>
-    <row r="30" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>312</v>
       </c>
@@ -4340,7 +4352,7 @@
       <c r="C30" s="49"/>
       <c r="D30" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="50"/>
       <c r="F30" s="51" t="s">
@@ -4364,7 +4376,9 @@
       <c r="V30" s="70"/>
       <c r="W30" s="55"/>
       <c r="X30" s="55"/>
-      <c r="Y30" s="94"/>
+      <c r="Y30" s="94">
+        <v>1</v>
+      </c>
       <c r="Z30" s="57"/>
       <c r="AA30" s="58"/>
       <c r="AB30" s="69"/>
@@ -4403,7 +4417,7 @@
       <c r="BI30" s="57"/>
       <c r="BJ30" s="58"/>
     </row>
-    <row r="31" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30">
         <v>40</v>
       </c>
@@ -4416,7 +4430,7 @@
       </c>
       <c r="D31" s="42">
         <f>SUM(D32:D35)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="31"/>
@@ -4477,7 +4491,7 @@
       <c r="BI31" s="74"/>
       <c r="BJ31" s="78"/>
     </row>
-    <row r="32" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>401</v>
       </c>
@@ -4489,7 +4503,7 @@
       </c>
       <c r="D32" s="83">
         <f>SUM(G32:BJ32)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E32" s="50"/>
       <c r="F32" s="51"/>
@@ -4530,7 +4544,9 @@
       <c r="AO32" s="58"/>
       <c r="AP32" s="53"/>
       <c r="AQ32" s="54"/>
-      <c r="AR32" s="55"/>
+      <c r="AR32" s="55">
+        <v>2</v>
+      </c>
       <c r="AS32" s="55"/>
       <c r="AT32" s="56"/>
       <c r="AU32" s="57"/>
@@ -4550,7 +4566,7 @@
       <c r="BI32" s="57"/>
       <c r="BJ32" s="58"/>
     </row>
-    <row r="33" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>402</v>
       </c>
@@ -4623,7 +4639,7 @@
       <c r="BI33" s="57"/>
       <c r="BJ33" s="58"/>
     </row>
-    <row r="34" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>403</v>
       </c>
@@ -4635,7 +4651,7 @@
       </c>
       <c r="D34" s="83">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E34" s="50"/>
       <c r="F34" s="51"/>
@@ -4676,7 +4692,9 @@
       <c r="AO34" s="58"/>
       <c r="AP34" s="59"/>
       <c r="AQ34" s="60"/>
-      <c r="AR34" s="55"/>
+      <c r="AR34" s="55">
+        <v>2</v>
+      </c>
       <c r="AS34" s="55"/>
       <c r="AT34" s="56"/>
       <c r="AU34" s="57"/>
@@ -4696,7 +4714,7 @@
       <c r="BI34" s="57"/>
       <c r="BJ34" s="58"/>
     </row>
-    <row r="35" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>404</v>
       </c>
@@ -4765,7 +4783,7 @@
       <c r="BI35" s="57"/>
       <c r="BJ35" s="58"/>
     </row>
-    <row r="36" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>50</v>
       </c>
@@ -4839,7 +4857,7 @@
       <c r="BI36" s="74"/>
       <c r="BJ36" s="78"/>
     </row>
-    <row r="37" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>501</v>
       </c>
@@ -4910,7 +4928,7 @@
       <c r="BI37" s="57"/>
       <c r="BJ37" s="58"/>
     </row>
-    <row r="38" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>502</v>
       </c>
@@ -4979,7 +4997,7 @@
       <c r="BI38" s="57"/>
       <c r="BJ38" s="58"/>
     </row>
-    <row r="39" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>60</v>
       </c>
@@ -5053,7 +5071,7 @@
       <c r="BI39" s="74"/>
       <c r="BJ39" s="78"/>
     </row>
-    <row r="40" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>601</v>
       </c>
@@ -5124,7 +5142,7 @@
       <c r="BI40" s="57"/>
       <c r="BJ40" s="58"/>
     </row>
-    <row r="41" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
         <v>602</v>
       </c>
@@ -5195,7 +5213,7 @@
       <c r="BI41" s="57"/>
       <c r="BJ41" s="58"/>
     </row>
-    <row r="42" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>603</v>
       </c>
@@ -5264,7 +5282,7 @@
       <c r="BI42" s="57"/>
       <c r="BJ42" s="58"/>
     </row>
-    <row r="43" spans="1:62" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:62" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="35"/>
       <c r="B43" s="36" t="s">
         <v>6</v>
@@ -5275,7 +5293,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5345,15 +5363,15 @@
       </c>
       <c r="W43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Z43" s="39">
         <f t="shared" si="3"/>
@@ -5429,7 +5447,7 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
@@ -5535,21 +5553,21 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="102" t="s">
         <v>13</v>
       </c>
@@ -5561,7 +5579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="100" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
@@ -5578,7 +5596,7 @@
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="100" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
@@ -5595,7 +5613,7 @@
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="100" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
@@ -5607,12 +5625,12 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="100" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
@@ -5624,11 +5642,11 @@
       </c>
       <c r="D6" s="80">
         <f>Zeitplanung!D31</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F6" s="81"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="100" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
@@ -5644,7 +5662,7 @@
       </c>
       <c r="F7" s="81"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="100" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
@@ -5660,7 +5678,7 @@
       </c>
       <c r="F8" s="81"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:6" ht="15.6" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A7:B7"/>
@@ -5672,7 +5690,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="56" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>